<commit_message>
table: Species change No variable to Str
</commit_message>
<xml_diff>
--- a/FC_tables/Species.xlsx
+++ b/FC_tables/Species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silver_Wolf\Documents\Rcourses\Fantacy_Craft\FC_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88625E2-6F0A-4A54-9882-38719488BD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76C09FE-9826-4357-88CB-799B3A75B602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,11 +838,14 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.85546875" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" customWidth="1"/>
     <col min="17" max="17" width="21.140625" customWidth="1"/>
@@ -1161,7 +1164,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1309,7 +1312,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1605,7 +1608,7 @@
         <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>